<commit_message>
improved the scraping script from recurrent navi
</commit_message>
<xml_diff>
--- a/try-my-hand/data/recurrent_navi_tyo.xlsx
+++ b/try-my-hand/data/recurrent_navi_tyo.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -493,801 +493,798 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>138389</t>
+          <t>155196</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>工学,対面講座</t>
+          <t>その他カルチャー,対面講座</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-02-15</t>
+          <t>2026-01-24</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2級管工事施工管理技士(一次・二次)受験対策</t>
+          <t>バレーボール観戦力養成講座</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/138389</t>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/155196</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>２級管工事施工管理技士受験対策
-(1)一般基礎、空調設備、衛生設備、施工管理
-(2)施工管理記述、空調設備記述、衛生設備記述、施工体験</t>
+          <t>【概容】
+バレーボールをさまざまな角度、視点からみる「観戦術」を学び、あらゆる側面をより深く知るための「観戦力」を高めましょう。これらの学習によりバレーボールIQを高め、選手として、サポーターとして、運営スタッフやボランティアとして、より良い成功や喜びを手にしてください。
+【本講座のねらい（到達目標）】
+バレーボールIQを高め、「する・見る・支える」スポーツの参加者としての素養を修得する。</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>多摩・島しょ部,北多摩エリア,昭島市</t>
+          <t>世田谷区</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>多摩職業能力開発センター</t>
+          <t>駒澤大学</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>20名</t>
+          <t>200名</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>3,200円</t>
+          <t>1,000円</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025年1月10日</t>
+          <t>2026年1月17日（土）23:59</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>137784</t>
+          <t>155194</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>工学,対面講座</t>
+          <t>その他カルチャー,対面講座</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-03-09</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第三種電気主任技術者科目合格対策(法規)</t>
+          <t>江戸日本橋の架橋と江戸周辺地域</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/137784</t>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/155194</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>第三種電気主任技術者試験(法規)受験対策
-電気事業法、電気設備技術基準、電気施設管理</t>
+          <t>【概容】
+五街道の起点とされる日本橋の歴史について再整理し、周辺地域との関係を述べていきます。特に、江戸東郊地域（深川・本所など）のあり方を取り上げます。この他、参勤交代の成立や江戸城総構えの成立にも言及します。
+【本講座のねらい（到達目標）】
+日本橋の歴史への理解を深め、その上で江戸時代の歴史を展望できる。</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>多摩・島しょ部,昭島市</t>
+          <t>世田谷区</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>多摩職業能力開発センター八王子校</t>
+          <t>駒澤大学</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>40名</t>
+          <t>200名</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>1,600円</t>
+          <t>1,000円</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025年1月10日</t>
+          <t>2025年12月13日（土）23:59</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>138428</t>
+          <t>155192</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>工学,対面講座</t>
+          <t>その他経済産業・社会,対面講座</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-03-02</t>
+          <t>2025-11-15</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第二種電気工事士(実技) 【初級】</t>
+          <t>初めて学ぶ著作権法</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/138428</t>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/155192</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>電気基礎、電気図記号、図面の見方、電気工事実習、第二種電気工事士受験ポイント</t>
+          <t>【概容】
+SNSの投稿やWebサイトの制作を行う際に、イラストや写真など他人の著作物の著作権を侵害していないか、不安に感じたことはありませんか。本講座では、著作権法を初めて学ぶ方を対象に、その基本的なルールをわかりやすく解説します。
+【本講座のねらい（到達目標）】
+インターネット上で情報を発信する際に、最低限守るべき著作権法の基本的なルールを理解する。</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>多摩・島しょ部,北多摩エリア,府中市</t>
+          <t>世田谷区</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>多摩職業能力開発センター府中校</t>
+          <t>駒澤大学</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>30名</t>
+          <t>200名</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>6,500円</t>
+          <t>1,000円</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025年1月10日</t>
+          <t>2025年11月8日（土）23:59</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>143983</t>
+          <t>155188</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>最先端技術,対面講座</t>
+          <t>その他経済産業・社会,オンデマンド講座</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-03-01</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Raspberry PI【初級】</t>
+          <t>食べることは生きること！</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/143983</t>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/155188</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>センサーによる信号を表示する一連の流れを理解し、実際に回路を作成する手順を習得する。</t>
+          <t>【概容】
+令和の米騒動をはじめとして食と農に対する世の中の関心が高まっています。食生活の大切さを学び、日本の農政・農業について紐解き、これからの食と農の在り方について一緒に考えましょう。
+【本講座のねらい（到達目標）】
+「人生100年」は健康であればこそ。日々の食事に関心を持ち、たべものを見つめ直すことにつなげてください。食と農に対する理解が深まり、自らの食生活や農業・環境・社会との関わりを考える契機となり、必要に応じて見直していく動機づけとなることを期待します。</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>多摩・島しょ部,北多摩エリア,昭島市</t>
+          <t>オンライン</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>多摩職業能力開発センター</t>
+          <t>駒澤大学</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>10名</t>
+          <t>400名</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>6,500円</t>
+          <t>4,000円</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025年1月10日</t>
+          <t>2026年1月18日（日）23:59</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>111975</t>
+          <t>155184</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>経済産業・社会,対面講座</t>
+          <t>その他経済産業・社会,オンデマンド講座</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-03-02</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>ホームページビルダーによるホームページ作成</t>
+          <t>事故と損害賠償</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/111975</t>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/155184</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>ホームページの基礎知識、Webサイトとトップページの作成および編集、リンクの設定、画像の作成と編集
-【ホーページビルダー21】</t>
+          <t>【概容】
+いろんな事例を挙げながら、事故が発生した場合に、どのようなことがあれば相手方に損害賠償を請求することができるかを考えます。また、損害賠償額はどのようにして定められるかを考えます。これらは、民法の中の重要な部分である不法行為の問題です。
+【本講座のねらい（到達目標）】
+相手方が損害賠償責任を負う場合について、また、損害賠償額を定めるときに考慮する事項について理解することができるようになる。</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>多摩・島しょ部,北多摩エリア,府中市</t>
+          <t>オンライン</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>多摩職業能力開発センター府中校</t>
+          <t>駒澤大学</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>25名</t>
+          <t>400名</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>6,500円</t>
+          <t>4,000円</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025年1月10日</t>
+          <t>2025年12月14日（日）23:59</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>74856</t>
+          <t>155180</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>工学,対面講座</t>
+          <t>その他経済産業・社会,オンデマンド講座</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2025-03-02</t>
+          <t>2025-11-04</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>リレーシーケンス制御【初級】</t>
+          <t>文化とグローバリゼーションの20世紀からの中・長期的展望</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/74856</t>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/155180</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>シーケンス図の読み方・書き方、タイムチャート図の読み方・書き方、制御機器の取扱い方、基本回路の組立配線</t>
+          <t>【概容】
+20世紀から21世紀の最初の四半世紀にかけて、グローバリゼーションが進行し、それに伴い、文化システムが大きく変化(トランスフォーメーション)してきました。本講座では、それを、その変化の中心を担ってきた、イギリス・アメリカ文化、シンガポール文化、中国文化、日本文化、に絞って、その変化の中・長期的概要を論じます。
+【本講座のねらい（到達目標）】
+本講座では、グローバルな秩序と文化システムの変化を、細部ではなく、全体的な枠組みを具体的に理解することを目標としている。</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>多摩・島しょ部,北多摩エリア,昭島市</t>
+          <t>オンライン</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>多摩職業能力開発センター</t>
+          <t>駒澤大学</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>20名</t>
+          <t>400名</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>6,500円</t>
+          <t>4,000円</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025年1月10日</t>
+          <t>2025年11月16日（日）23:59</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>143959</t>
+          <t>155169</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>経済産業・社会,対面講座</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>2025-03-03</t>
-        </is>
-      </c>
+          <t>その他最先端技術,オンデマンド講座</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>宅建業・不動産業就職科（吉祥寺）</t>
+          <t>『ChatGPT×マーケティングの教科書』出版記念 生成AIをマーケティングで徹底活用！‐ 分析から戦略立案まで独力で実現する ‐</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/143959</t>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/155169</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>コースの内容
-当訓練では4か月かけてFP3級の基礎を理解し、宅地建物取引士の試験を受験できるスキルを身に付けます。不動産業で働く際、その事務所ごと5人に1人以上必要とされている宅地建物取引士の資格取得に必要な法知識を習得するため、初学者向けに各法令を反復して学習します。FP3級は金融系、保険系、不動産系、建築系など幅広い分野で活躍できる資格です。業界未経験者も想定し、FP3級では基礎的なお金の知識について学習します。日々の就職支援として隔週で求人情報の提供を行い、常に最新の情報を得られる環境の中で、就職活動や授業内容など講師への質問もしやすい体制を整えております。企業説明会も職業訓練修了生を積極的に採用する企業を中心に４社～ 5社実施いたします。アットホームな雰囲気で講師との距離も近く、事務局とのコミュニケーションも取りやすい環境です。
-                                                                                                                                                                                                                                                                                                                                                                                                                                  ※本講座は3/3～6/30の期間を通じて行われます。</t>
+          <t>現在、生成AIのビジネス活用は急速に広まっています。しかし、戦略立案、データ分析、ビジネスアイデアの創出といった高度なレベルでの活用は、まだ出発点に立ったばかりです。本セミナーでは、ChatGPTを活用したマーケティングの具体的なステップや戦略立案の方法をご紹介。本書をまだお読みでない方向けに基本から丁寧に解説しますが、事前にお読みいただくと、より理解が深まります。</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>多摩・島しょ部,北多摩エリア,武蔵野市</t>
+          <t>オンライン</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>東京都（実施機関） 日建学院吉祥寺校</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>20名</t>
-        </is>
-      </c>
+          <t>サイバー大学</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr">
         <is>
-          <t>無料（別途、教科書代等は本人負担となります。）</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>2025年1月17日</t>
-        </is>
-      </c>
+          <t>無料</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>143955</t>
+          <t>155164</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>経済産業・社会,オンデマンド講座,対面講座</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>2025-02-26</t>
-        </is>
-      </c>
+          <t>その他ビジネススキル,オンデマンド講座</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>食育講座「簡単リメイクレシピをご紹介！“もったいない”をなくす食べきりテクニック」</t>
+          <t>マーケティングの当たり前を疑う</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/143955</t>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/155164</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>少しだけ残った大切な食材、もったいないですね。この講座では、簡単リメイクでおいしく食べきるオリジナルレシピをご紹介。
-ムダなく買ってきちんと使い切り、楽しみながらおいしくリメイクしましょう！</t>
+          <t>商品開発や販売促進といったマーケティングの実践現場に身を置いていると、多くのマーケッターが「当たり前」と信じていること、「正解」と疑わずにいることのなかに、実は間違いが潜んでいるのではないかと感じること、しばしばです。
+マーケティングの「研究」「実践」の両軸に携わる立場から、今回は「3つの当たり前を疑う」をテーマに解説します。</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>オンライン,多摩・島しょ部,北多摩エリア,立川市</t>
+          <t>オンライン</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>多摩消費生活センター</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>(集合講座）定員１８名(18歳以上)  (オンデマンド講座）定員なし</t>
-        </is>
-      </c>
+          <t>サイバー大学</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr">
         <is>
           <t>無料</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>(集合講座）2025年2月3日（月）正午  (オンデマンド講座）2025年3月20日（木・祝）</t>
-        </is>
-      </c>
+      <c r="K9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>143952</t>
+          <t>155157</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>経済産業・社会,オンデマンド講座</t>
+          <t>建築工学,芸術・アート,ライフスタイル・現代文化,対面講座</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2024-12-27</t>
+          <t>2025-11-22</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>偽　デジタル広告への対応と消費者力</t>
+          <t>生活や仕事に活かす色彩入門講座 &lt;色を楽しく学び、役立てる&gt;</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/143952</t>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/155157</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>インターネット上には、見分けのつかない偽・誤情報や不正広告等が溢れ、情報の信憑性を見抜くことが難しくなってきています。消費者・事業者・行政がそれぞれの取組を紹介し、私たちがどう対応していくかを考えます。</t>
+          <t>配色力を向上したい人に向けた「使える色彩」講座です。
+デザインのあらゆる創作活動のベースとなる配色力を、日本カラーデザイン研究所と ICS カレッジオブアーツのオリジナル教材を使用して、徹底的に身につけます。
+実習中心のカリキュラムで、美しく説得力のある配色や、オリジナリティのある配色を実践的に学習。
+「配色テクニック」の習得と「センスアップ」の両方を目指せる講座です。</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>オンライン</t>
+          <t>目黒区</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>東京都消費生活総合センター</t>
+          <t>専門学校ICSカレッジオブアーツ</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>無し</t>
+          <t>20名</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>無料</t>
+          <t>120,000円</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>無し</t>
+          <t>2025年11月19日（水）</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>143948</t>
+          <t>155152</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>経済産業・社会,対面講座</t>
+          <t>建築工学,芸術・アート,ライフスタイル・現代文化,対面講座</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2025-02-14</t>
+          <t>2025-11-22</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>～消費者被害の未然防止～　神楽河岸寄席</t>
+          <t>ベーシック「コーディネーション基礎」（土曜コース）</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/143948</t>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/155152</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>出前寄席事業は、ご用命に応じて、学校や高齢者施設に出向き、消費者被害の未然防止に役立つ情報をお届けしています。
-このたび、新作を作成しましたので、ご披露いたします。</t>
+          <t>基礎知識のレクチャー、空間分析やマテリアル分析の方法、マテリアルのリサーチ手法・選び方、プレゼンテーショボード作成など、インテリアコーディネーションを行う上で必要となる基本的な知識やスキルを習得できる講座です。</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>23区,都心・副都心エリア,新宿区</t>
+          <t>目黒区</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>東京都消費生活総合センター</t>
+          <t>専門学校ICSカレッジオブアーツ</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>100名</t>
+          <t>20名</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>無料</t>
+          <t>100,000円</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025年2月3日</t>
+          <t>2025年11月19日（水）</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>142928</t>
+          <t>155147</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>経済産業・社会,オンデマンド講座</t>
+          <t>建築工学,芸術・アート,ライフスタイル・現代文化,対面講座</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2024-11-25</t>
+          <t>2025-11-19</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>メインシンポジウム「だまし被害にあわない！　デジタル社会を生きる力」オンライン配信</t>
+          <t>レジデンス「寝室のスタイル」</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/142928</t>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/155147</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>生成AIの発達などに伴いだましの手口も進化し、デジタル社会における消費者被害はますます増加しています。詐欺・悪徳商法の心理学研究の第一人者として活躍されている立正大学心理学部教授の西田公昭さんを講師に迎え、私たち消費者がデジタル社会で賢く生きる知恵をお話しいただきました。講演会の録画を期間限定で配信します。</t>
+          <t>住宅の生活空間のスタイルコーディネーションを、レクチャーと実習を中心に学ぶ、プロのための講座です。自分のスタイルを見つけたい、よりハイエンドのスタイルを学びたい経験者におすすめです。
+今回のテーマは「寝室」
+住宅の中で最もプライベートな空間で、クライアントのライフスタイルが現れる場です。既成の家具や仕上げにとらわれない寝室のエレメントの選び方、造作の方法を実践的に学びます。
+実物のサンプルを用いて、色・質感・仕上げの組み合わせを検討し、マテリアルボードの制作を行います。
+講師:横堀健一
+ハイエンドな個人邸の設計やマンションデザイン監修などで高い評価を得る建築家。Organicmodernをコンセプトに、自然と建築の調和を大切にしながら、「古典と現代、西洋と東洋が融合する」唯一無二の空間を想像し続けています。建築をインテリアデザインやデコレーション、アートの視点から総合的にとらえ、クライアントから高い満足と信頼を得ています。
+講師:コマタトモコ
+住宅、店舗、ショールームなどハイエンドなインテリアデザインで定評のあるインテリアデザイナー。「人と場の物語と歴史」を大切にしながら、唯一無二の住空間を創造し続けています。素材や色彩の調和、家具や照明の配置、空間全体のストーリー性を巧みに組み立てるコーディネーションで定評があります。国内外のデザイン潮流にも精通し、時代や国境を超え、空間と家具とアートを融合したボーダレスな空間を創造します。</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>オンライン</t>
+          <t>目黒区</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>東京都消費者月間実行委員会</t>
+          <t>専門学校ICSカレッジオブアーツ</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>なし</t>
+          <t>20名</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>無料</t>
+          <t>120,000円</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>なし</t>
+          <t>2025年11月16日（日）</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>141737</t>
+          <t>155142</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>経済産業・社会,対面講座</t>
+          <t>建築工学,芸術・アート,ライフスタイル・現代文化,対面講座</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2025-03-03</t>
+          <t>2025-11-15</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>ビジネスソフト実践科</t>
+          <t>日常と非日常が交差する宿泊空間のためのインテリアスタイリング</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/141737</t>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/155142</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>コースの内容
-WordやExcelをMOS資格取得レベルまで、またPowerPointの基礎も習得し、業務で活かせるスキルを身に付けます。オリジナルの教材と市販の教材を使用して基礎からしっかりステップアップしていきます。さらに、実務を想定した演習問題で実践力を養います。各種試験会場になっているので、慣れた環境で効率よく受験が可能です。就職支援ではキャリアコンサルタントが常駐しているので、就職相談、応募書類の添削や模擬面接も個別で随時対応します。また、採用実績のある企業の説明会等を実施します。訓練初期から就職に向けての行動計画を立て、スキルを習得しつつ就職に向けて早期に行動するよう促します。駅からも学校からも近い託児施設と契約しているため、希望者の方（条件有り）は安心してお子様を預けて学習に専念することができます。
-                                                                                                                                                                                                                                                                                                                                                                                                                           ※本講座は3/3～5/30の期間を通じて行われます。</t>
+          <t>ホテルでも住宅でもない、「民泊」という場に求められるスタイリングとは何か。
+都内に実在する高級民泊を舞台に、現地見学と演習を通じて空間のコンセプトづくりからスタイリングまでを実践的に学びます。
+住むように街の日常を感じ、旅先でしか得られない非日常の高揚感を味わう。そのような民泊特有の体験を支える空間の魅力づくりを学びたい経験者におすすめの講座です。
+講師:守 真史
+今回の舞台となる民泊の空間デザインを担当したインテリアスタイリスト。
+内装設計から装飾小物のスタイリング、オリジナルプロダクトの制作まで、日常生活のなかに少しだけ祝祭的な非日常を感じさせるような空間や物のデザインを行っています。</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>多摩・島しょ部,北多摩エリア,武蔵野市</t>
+          <t>目黒区</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>東京都（実施機関） 専門学校中野スクールオブビジネス</t>
+          <t>専門学校ICSカレッジオブアーツ</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>30名</t>
+          <t>20名</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>無料（別途、教科書代等は本人負担となります。）</t>
+          <t>120,000円</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025年1月17日</t>
+          <t>2025年11月12日（水）</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>139711</t>
+          <t>155129</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>経済産業・社会,オンライン講座</t>
+          <t>社会,対面講座</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2025-03-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>総務・経理就職（オンライン）科</t>
+          <t>食と農セミナー「コメ農家が伝えるこれまでの挑戦と今後の展望」</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/139711</t>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/155129</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>コースの内容
-再就職が円滑に進むよう、育児等と両立しやすいオンライン訓練を中心とした短時間コースです。総務職に必要な労働保険・社会保険の知識や経理職に必要な簿記、源泉徴収の知識を学習します。さらに会計ソフト（弥生会計）と給与計算ソフト（弥生給与）、Microsoft Excel/ Word 2019の操作技能を習得することで、企業の総務・経理部門、会計事務所、社労士事務所への就職を目指します。
-※本講座は3/3～6/30の期間を通じて行われます。</t>
+          <t>800年続くコメ農家の横田修一さんを講師に迎え、日本の食料安全保障の要と言われている「米」の生産者が今置かれている状況やその背景、横田農場の取り組みや成果をお聞きします。農業や食について考えましょう。</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>23区,千代田区,都心・副都心エリア</t>
+          <t>千代田区</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>東京都（実施機関） 大原簿記学校3号館</t>
+          <t>東京都消費者月間実行委員会</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>25名</t>
+          <t>100名</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>無料（別途、教科書代等は本人負担となります。）</t>
+          <t>無料</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025年1月17日</t>
+          <t>2025年11月24日（月）23:59</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>138097</t>
+          <t>154688</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>医療・福祉,対面講座</t>
+          <t>その他経済産業・社会,オンライン講座</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2025-02-01</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>保育士就職支援セミナー　第７回</t>
+          <t>食育講座「旬の恵みを島からも畑からも！～東京の地産地消～」</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/138097</t>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/154688</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>保育の専門知識や保護者対応など、保育の仕事に活かせる実践的なプログラムを学べる２日間のセミナーです。
-セミナー受講者のうち、希望する方は保育所での実習にご参加いただけます。</t>
+          <t>立川市内で地場野菜と小笠原食材を使った飲食店を経営する講師をお迎えし、広く「東京の地産地消」について学べる講座です。お家でできる簡単レシピも紹介します。</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>23区,台東区,城東エリア</t>
+          <t>オンライン</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>東京都保育人材・保育所支援センター</t>
+          <t>東京都多摩消費生活センター</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>40名</t>
+          <t>定員なし</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -1297,55 +1294,55 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>令和７年１月22日（水）</t>
+          <t>2026年1月29日（木）23:59</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>138092</t>
+          <t>155117</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>医療・福祉,対面講座</t>
+          <t>その他最先端技術,その他自然科学,オンライン講座</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2025-01-18</t>
+          <t>2025-11-08</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>保育士就職支援セミナー　第６回</t>
+          <t>2025年度 社会人アカデミー講演会「東京科学大学研究者が構想する未来の医工連携」</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/138092</t>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/155117</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>保育の専門知識や保護者対応など、保育の仕事に活かせる実践的なプログラムを学べる２日間のセミナーです。
-セミナー受講者のうち、希望する方は保育所での実習にご参加いただけます。</t>
+          <t>東京科学大学（Science Tokyo）社会人アカデミーは、本学教員同士の対談による講演会「東京科学大学研究者が構想する未来の医工連携」を開催します。本講演会は、東京科学大学社会人アカデミーとして統合後、二度目の開催となり、医療分野と工学分野の連携に関する展望も内容に含めた画期的な講演プログラムとなっております。
+研究者の学問的区分を超えた総合的な知を通して、人類社会の現在、そして未来を大胆に展望します。</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>23区,城南エリア,大田区</t>
+          <t>オンライン</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>東京都保育人材・保育所支援センター</t>
+          <t>東京科学大学社会人アカデミー、蔵前工業会　共催</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>40名</t>
+          <t>150名</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -1355,50 +1352,55 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>令和７年１月８日（水）</t>
+          <t>2025年11月3日（月）23:59</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>136746</t>
+          <t>155107</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>経済産業・社会,オンライン講座,対面講座</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr"/>
+          <t>その他自然科学,オンライン講座</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2025-11-05</t>
+        </is>
+      </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>高齢者見守り人材向け出前講座</t>
+          <t>Science Tokyo(tip)発無料オンライン企画！『ヒトの加齢性変化を「形」から観る：骨盤底と股関節の筋の研究事例』</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/136746</t>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/155107</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>高齢者を狙う悪質商法の手口と対処法、見守りのポイント、被害発見時の対応などを消費生活相談の経験を持つ相談員が講師となりわかりやすくお伝えします。</t>
+          <t>東京科学大学 tipより無料オンラインセミナー（tip BBセミナー）をご案内します。
+Science Tokyoおよびtip会員（産学官）発の現場の課題や連携ニーズを発信しますので、課題解決の糸口を探す場としてご活用ください！</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>オンライン,23区,多摩・島しょ部</t>
+          <t>オンライン</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>申込者</t>
+          <t>東京科学大学　医療イノベーション機構　tip BBセミナー事務局</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>原則 10名以上</t>
+          <t>なし</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -1408,55 +1410,55 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>遅くても希望日の1か月前</t>
+          <t>2025年11月5日  18:00</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>136726</t>
+          <t>155095</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>経済産業・社会,オンライン講座,対面講座</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr"/>
+          <t>AI・機械学習,社会,対面講座</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2025-10-21</t>
+        </is>
+      </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>学校向け出前講座</t>
+          <t>成蹊大学Society 5.0研究所主催第18回講演会「現実×仮想の世界における法律:未来の世界で何が起きるか？」</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/136726</t>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/155095</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>消費生活相談や商品テスト指導などの経験を積んだ東京都消費者啓発員（コンシューマー・エイド）が、悪質商法被害の実例に基づき、被害防止の方法・対策について、詳しく解説いたします。
-・契約とは何か／成年年齢引き下げに伴う消費者としての心得
-・悪質商法被害防止（マルチ商法・定期購入など）
-・インターネットやSNSのトラブル防止
-・お金の使い方（キャッシュレス、ローンやクレジットの仕組み）
-・糖度の測定（実験講座）</t>
+          <t>技術の発展に伴って、メタバースという新たな空間の例のように、現実と仮想が交錯する時代が訪れた。これに伴う新しい法律問題はどのように解決されるのだろうか。このようなバーチャル空間で何かを「所有」することはできるのか？別の誰かと喧嘩するなどの問題が起きたらどうするか？
+エンタテインメントやファッションに加え、クロスリアリティ（XR）・メタバース、VTuber、人工知能（AI）、eSportsといった先端テクノロジー関係の法務についての日本屈指の専門家から、デジタル×社会の展望やそこで生じる法律問題などについて、幅広いトピックについて解説いただきます。</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>オンライン,23区,多摩・島しょ部</t>
+          <t>武蔵野市</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>申込者</t>
+          <t>成蹊大学Society 5.0研究所</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>原則 10名以上</t>
+          <t>約90名</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -1466,146 +1468,156 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>遅くても希望日の1か月前</t>
+          <t>2025年10月21日15:00</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>83980</t>
+          <t>154548</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>経済産業・社会,対面講座</t>
+          <t>経済,産業,社会,オンライン講座</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2025-03-08</t>
+          <t>2025-11-08</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>WordPressによるWebサイト制作</t>
+          <t>法政大学大学院 地域創造インスティテュート2025年4月創設記念 公開講座『越境学習とリカレント教育』</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/83980</t>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/154548</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>WordPressの概要、システムの構成、作業の概要、WordPressの設定、テーマ(テンプレート)の作成、プラグインの作成</t>
+          <t>講師　石山  恒貴（いしやま　のぶたか） 法政大学大学院地域創造インスティテュート教授
+  近年、注目を集める越境学習。その対象は、あらゆる年代に及びます。言い換えれば、越境学習とは生涯を通じた学びなのです。すなわち、越境学習はリカレント教育と密接な関係にあります。本講座では、越境学習の特徴、意義を明らかにし、リカレント教育との共通性を明確にします。さらに越境学習とリカレント教育の課題と今後の方向性を述べていきます。</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>23区,北区,城北エリア</t>
+          <t>オンライン</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>中央・城北職業能力開発センター赤羽校</t>
+          <t>法政大学</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>29名</t>
+          <t>150名</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>6,500円</t>
+          <t>無料</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2024年12月10日</t>
+          <t>2025年11月4日（火）17時</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>62289</t>
+          <t>154945</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ビジネススキル,工学,医療・福祉,オンライン講座,対面講座</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr"/>
+          <t>電気・電子工学,オンライン講座</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2026-01-06</t>
+        </is>
+      </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>短期集中型資格取得支援訓練</t>
+          <t>第三種電気主任技術者科目合格対策(機械)</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/62289</t>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/154945</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>東京都は、求職中の方などに対し、短期間で成長産業分野等に関連する資格を取得していただくことで、早期の再就職を支援するため、eラーニングによる学習と、宿泊を伴う試験直前期の集合型講習を組み合わせた訓練を実施します。
-　eラーニングで基礎的な知識を習得していただき、試験直前期の集合型講習で、過去問演習などに集中的に取り組んでいただくことで、短期間での資格取得をサポートいたします。</t>
+          <t>第三種電気主任技術者科目合格対策(機械)
+電気機器、パワエレ、自動制御、照明、他</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>オンライン,豊島区</t>
+          <t>オンライン</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>東京都</t>
+          <t>東京都立中央・城北職業能力開発センター</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>備考欄に記載の事業ホームページを参照ください。</t>
+          <t>50名</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>受講料及び集合型講習における宿泊費は無料 （資格試験等の受験料や集合型講習会場までの交通費、集合型講習期間中の食費は自己負担となります。）</t>
+          <t>2400円</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>定員に達し次第、募集を締め切ります。</t>
+          <t>2025年10月25日（土）23:59</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>48165</t>
+          <t>154940</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>ビジネススキル,オンライン講座</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr"/>
+          <t>建築工学,オンライン講座</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2026-01-13</t>
+        </is>
+      </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>成長産業分野キャリア形成支援事業</t>
+          <t>二級建築士(学科・施工)受験対策</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/48165</t>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/154940</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>非正規労働者等へキャリア形成の機会を提供し、雇用の安定化と成長産業分野への人材シフトを促進するため、eラーニング等による新たな資格やスキルの取得支援及び職業紹介等の就職支援を一体的に行う事業です。</t>
+          <t>二級建築士(学科・施工)受験対策
+建築施工、測量積算、演習解説</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1615,161 +1627,168 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>東京都</t>
+          <t>東京都立中央・城北職業能力開発センター</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>備考欄に記載の事業ホームページを参照ください。</t>
+          <t>50名</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>原則無料（通信費のみ自己負担）でご受講いただけます。</t>
+          <t>1600円</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>定員に達し次第、募集を締め切ります。</t>
+          <t>2025年10月25日（土）23:59</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>16796</t>
+          <t>154935</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>経済産業・社会,オンライン講座,対面講座</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr"/>
+          <t>その他経済産業・社会,オンライン講座</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2026-02-07</t>
+        </is>
+      </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>出前寄席</t>
+          <t>ITパスポート試験受験対策(テクノロジ系)</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/16796</t>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/154935</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>悪質商法の手口とその対処法など消費者被害の未然防止に役立つ情報を、落語・漫才・コントで楽しく、わかりやすくお伝えします。</t>
+          <t>IT パスポート試験詳細、インターネット、マルウェア、暗号化技術、情報セキュリティ管理、ディジタルとアナログ、マルチメディアの表現と論理、アルゴリズムとデータ構造、プログラミング、IoTとAIコンピュータのハードウェア、システム構成、コンピュータのソフトウェア、データベース、過去問題演習</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>オンライン,23区,多摩・島しょ部</t>
+          <t>オンライン</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>申込者</t>
+          <t>東京都立中央・城北職業能力開発センター</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>原則10名以上</t>
+          <t>50名</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>6,700円～</t>
+          <t>1600円</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>遅くても希望日の1か月前</t>
+          <t>2025年10月25日（土）23:59</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>16742</t>
+          <t>154930</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>経済産業・社会,オンライン講座,対面講座</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr"/>
+          <t>その他経済産業・社会,オンライン講座</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>出前講座</t>
+          <t>ITパスポート試験受験対策(ストラテジ系・マネジメント系)</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/16742</t>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/154930</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>東京都消費者啓発員（コンシューマー・エイド）がみなさんの企画するイベントや集会、研修会などに講師として伺い、消費生活に関する情報をわかりやすくお伝えします。</t>
+          <t>ストラテジ(企業と組織、企業と会計、分析手法と予測値、知的財産権、セキュリティ関連法規、標準化、経営戦略、ビジネスインダストリ、システム戦略)、マネジメント(システムのライフサイクル、システム開発プロセス、テストと保守、プロジェクトマネジメント、ITサービスマネジメント、システム監査と内部統制)、過去問題演習</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>オンライン,23区,多摩・島しょ部</t>
+          <t>オンライン</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>申込者</t>
+          <t>東京都立中央・城北職業能力開発センター</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>原則10名以上</t>
+          <t>50名</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>9,500円／時間～</t>
+          <t>1600円</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>遅くても希望日の1か月前</t>
+          <t>2025年10月25日（土）23:59</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>1850</t>
+          <t>154925</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>語学,オンデマンド講座</t>
+          <t>データサイエンス,オンライン講座</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2022-03-26</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>TOKYO ENGLISH CHANNEL ドキュメンタリー動画</t>
+          <t>データサイエンスのための統計学(応用編)</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/1850</t>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/154925</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>英語での会話や議論を通じて「使える英語力」の向上を目的とした動画学習コンテンツです。
-（TOKYO ENGLISH CHANNEL では、主に小学生、中学生、高校生からを対象とした英語を用いています。）</t>
+          <t>現実のデータには複数の要因があり複雑である。これを解析する方法が多変量解析である。講習では重回帰分析、ロジスティック判別など多変量解析を学び、ニューラルネットワークなど現在の機械学習の理解につなげていく。</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -1779,51 +1798,54 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>東京都</t>
+          <t>東京都立中央・城北職業能力開発センター</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>なし</t>
+          <t>50名</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>無料</t>
+          <t>1600円</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>なし</t>
+          <t>2025年10月25日（土）23:59</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>1848</t>
+          <t>154921</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>語学,オンデマンド講座</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr"/>
+          <t>データサイエンス,オンライン講座</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>2026-01-09</t>
+        </is>
+      </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>TOKYO ENGLISH CHANNEL コミュニケーションに役立つ動画</t>
+          <t>システム開発の基礎</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/1848</t>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/154921</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>英語のコミュニケーションに役立つフレーズが満載です。
-（TOKYO ENGLISH CHANNEL では、主に小学生、中学生、高校生からを対象とした英語を用いています。）</t>
+          <t>システム開発の概要、プログラミングとデータベースの各工程、プログラミングとデータベースの基礎、各種アプリケーションの運用</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -1833,52 +1855,54 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>東京都</t>
+          <t>東京都立中央・城北職業能力開発センター</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>なし</t>
+          <t>50名</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>無料</t>
+          <t>1000円</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>なし</t>
+          <t>2025年10月25日（土）23:59</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>1846</t>
+          <t>154917</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>語学,オンデマンド講座</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr"/>
+          <t>その他ビジネススキル,オンライン講座</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>2026-01-16</t>
+        </is>
+      </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>TOKYO ENGLISH CHANNEL バーチャル留学動画</t>
+          <t>建設業法の基礎</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/1846</t>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/154917</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>「バーチャル留学」の準備や参加後の復習に役立つ動画です。
-イベントの参加を問わず、グローバルな視点を広げる内容になっています。
-（TOKYO ENGLISH CHANNEL では、主に小学生、中学生、高校生からを対象とした英語を用いています。）</t>
+          <t>建設業法、建設業関連法令(民法、労働法、労働基準法、労働安全衛生法など)、請負契約</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -1888,67 +1912,71 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>東京都</t>
+          <t>東京都立中央・城北職業能力開発センター</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>なし</t>
+          <t>50名</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>無料</t>
+          <t>1000円</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>なし</t>
+          <t>2025年10月25日（土）23:59</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>1844</t>
+          <t>154712</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>語学,オンデマンド講座</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr"/>
+          <t>AI・機械学習,対面講座</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>2025-10-25</t>
+        </is>
+      </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>TokyoGlobalStudio -Intermediate-「テーマにそって探究してみよう」</t>
+          <t>「生成AIと創る新たな社会」</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/1844</t>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/154712</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>文理融合やSTEAMを意識した幅広いテーマ設定によるレクチャーやディスカッションを通じて、英語を使って探究的に学ぶことができます。 東京都教育委員会が「教育に関する覚書」等で連携している国内外の大学や行政機関等によるハイレベルな内容に触れることができます。
-動画に出てくる単語を学ぶ音声資料や一覧表、レクチャーの理解を深めるためのワークシートも添付しています。
--全20本配信-（主に高校生からを対象とした英語）</t>
+          <t>文章や画像を高速生成する「生成AI」は、社会構造を大きく変える可能性を秘めています。それに伴い、雇用の変化や社会システムの再編は、私たち一人ひとりが向き合うべき喫緊の課題です。この変革期において、私たちは何を学び、どう社会を創っていくべきか。
+　本シンポジウムでは、物事の本質を探究する「理学」の視点から生成AIの可能性と限界を深く理解し、変化に適応するための学びを支える「リカレント教育」の視点から、人間ならではの価値を発揮しながらAIと共存するための方策を探り
+ます。生成AIと共に創る未来社会への道しるべを、皆さまと共に見出す機会となることを願っております。</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>オンライン</t>
+          <t>文京区</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>東京都</t>
+          <t>日本女子大学</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>なし</t>
+          <t>－</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -1958,37 +1986,44 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>なし</t>
+          <t>2025年10月25日AM10:00</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>1842</t>
+          <t>154701</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>語学,オンデマンド講座</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr"/>
+          <t>福祉,オンデマンド講座</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>2025-09-25</t>
+        </is>
+      </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>TokyoGlobalStudio -Basic- 「役に立つ表現を文法と合わせて学習してみよう」</t>
+          <t>令和7年度ひきこもりに関する講演会をオンラインで配信します</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/1842</t>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/154701</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>具体的な使用場面でのドラマを通じて、役に立つ表現を、中学校で習う主な文法項目とともに学びます。理解を深め、定着を目指すワークシートもついています。
-動画の後半では、音読する・質問に答えるなど、「話すこと」をトレーニングできます。
--全40本配信-（主に中年生からを対象とした英語）</t>
+          <t>「どうしてこんなことに…」「何をどうすればいいのか分からない」
+ひきこもりの方を支える中で、そんな思いを抱えていませんか？
+今年度のオンライン講演会では、講師と元ひきこもり当事者2名による座談会を初開催。
+実際の体験談から、家族との関係や支援との出会い、回復への道のりを共有します。
+精神科医講師からは“今できること”のヒントも紹介。
+少しだけ心が軽くなる時間を過ごしてみませんか。</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -2020,44 +2055,48 @@
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>1840</t>
+          <t>154685</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>語学,オンデマンド講座</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr"/>
+          <t>社会,対面講座</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>2025-11-21</t>
+        </is>
+      </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>TokyoGlobalStudio -Elementary- 「基本的な語やフレーズを学んでみよう」</t>
+          <t>消費生活と「AI×SDGs」～ちょっと先の私たちの生活～</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/1840</t>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/154685</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>小学校外国語の教科書で扱われる主要フレーズ・単語を場面に即したやり取りを通じて、楽しく学びます。動画で学習した単語や英文をなぞる、写すなど、英文を「書くこと」を扱ったワークシートがついています。
--全18本配信-（主に小学５・６年生からを対象とした英語）</t>
+          <t>AI（人工知能）が進化を続け、社会のあらゆる分野で利用されています。
+私たちの暮らしにAIがもたらす影響について、SDGｓの観点も踏まえ、皆さんと一緒に考える講座です。</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>オンライン</t>
+          <t>渋谷区</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>東京都</t>
+          <t>東京都消費生活総合センター</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>なし</t>
+          <t>150名</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
@@ -2067,62 +2106,1353 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>なし</t>
+          <t>2025年11月11日（火）23:59</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>1835</t>
+          <t>154612</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>語学,オンデマンド講座</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr"/>
+          <t>その他医療・福祉,対面講座</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>2026-02-07</t>
+        </is>
+      </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>TokyoGlobalStudio -Beginner- 「英語の楽しさにふれてみよう」</t>
+          <t>シミュレーションで学ぶICUリハビリテーション ～体験して学び直し～</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/1835</t>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/154612</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>文部科学省教材「Let’s Try!」で扱われている主要フレーズ・単語を、歌やチャンツ、ゲーム、クイズ等を通じて、楽しく学びます。
- 動画の後半には、アルファベットを学ぶコーナーもあります。
--全18本配信-（主に小学３・４年生からを対象とした英語）</t>
+          <t>職種を問わず、ICUでリハビリテーション業務をする医療従事者を対象に、実際に体験しながらシミュレーションを通して知識を深める講座です。昭和医科大学教育研修棟シミュレーション室にて、最新シミュレーターや人工呼吸器に触れ、集中治療室で行われる高度急性期医療の中でリハビリテーション業務を実践していくための知識と実践力を養います。集中治療医やリハビリテーション医、看護師、臨床工学技士、理学療法士、作業療法士による多職種チームの講師陣とともに学修していきます。
+本講座は3学会合同呼吸療法認定士の認定更新講習会(50点)に指定されています。
+◆対象
+・ICUでリハビリテーション業務に携わる医療従事者 
+※職種は問いません</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
+          <t>品川区</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>昭和医科大学リカレントカレッジ</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>10名</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>18,000円</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>2026年1月20日（火）</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>154607</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>その他カルチャー,対面講座</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>2026-02-05</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>基本から解説!スマホで楽しむ写真教室</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/154607</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>何気なく撮っている写真から卒業しましょう。ワンランク上の作品に仕上げるための基礎を学び、実践する講座です。写真の知識が無くても大丈夫です!講師が丁寧に教えます。スマートフォンでも一眼カメラでも、 どちらにも活用できる撮影方法や技術を楽しく学びましょう。
+◆対象
+・スマホ、一眼カメラでの写真撮影に興味がある方
+・自然が好きな方
+・写真の基礎を学びたい方</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>品川区</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>昭和医科大学リカレントカレッジ</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>10名</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>10,000円</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>2026年1月20日（火）</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>154602</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>その他医療・福祉,対面講座</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>2026-01-21</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>動きやすさを追求する!3日間実践講座</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/154602</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>本講座では、膝関節のみならず、股関節や足関節など下半身の複数の関節に着目し、それらの連動性を高めることで、膝への負担を軽減し動作全体をスムーズにすることを目指します。動きやすさを追求することで、運動機能の向上や、日常生活の質の改善につなげます。テニスや登山、旅行など、やりたいことを自信をもって楽しめるからだづくりを始めましょう!
+◆対象
+・膝に問題を抱えている方
+・膝に不安がある方
+・膝の痛みや動きの硬さに悩んでいる方
+・歩き方や立ち上がり、階段動作に不安を抱えている方 
+・腰痛や姿勢の悪さに悩んでいる方 
+・旅行や運動を楽しみたいのに膝や足に自信がない方
+・将来的な健康のために、今から体のケアに取り組みたい方</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>品川区</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>昭和医科大学リカレントカレッジ</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>12名</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>10,000円</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>2025年12月20日（土）</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>154598</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>その他医療・福祉,対面講座</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>2026-01-21</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>60歳になったら始めよう!姿勢・歩き方実践講座</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/154598</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>自分史上最高に綺麗な姿勢、綺麗な歩き方を手に入れる講座です。動きの基本である姿勢・歩き方では、下肢の安定性が重要です。
+本講座は、特に足関節、足趾の機能を高めることで、骨格を支えるインナーマッスルを強化し、安定した体幹をつくります。バランスのとれた自分本来の美しいボディーラインの実現とカラダの動きを美しくコントロールするという行動変容により、自己肯定感が高まり、ストレスに負けないココロの軸をつくることができます。「美しいカラダの動かし方」を意識することで、自分磨きの時間にしていきましょう!
+◆対象
+・中高齢者で健康寿命を延ばし、身体つくりを目指したいと考えている方
+・現在の体力に自信がない方
+・洋服が綺麗に着こなせなくなった方
+・前向きな気持ちになれなくなった方
+・下腹が出てきた方
+・猫背になってきた方
+・腰回りが大きくなった方
+・疲れやすくなった方
+・外出する機会が減り、膝や腰が弱ってきた方
+・肩や首が凝るようになった方</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>品川区</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>昭和医科大学リカレントカレッジ</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>12名</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>10,000円</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>2025年12月20日（土）</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>154594</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>その他カルチャー,対面講座</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>2026-01-15</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>楽しく高める自然治癒力 ～セルフケアで免疫力アップ～</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/154594</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>ストレス過多な時代を生き抜くためには適度なリラックスや息抜きが必要です。本講座ではリラックスを生活の中に取り入れ、楽しみながら免疫力を高める方法を学んでいきます。マインドフルネス、野菜やハーブなどから健康や癒しを受け取る植物療法、認知症予防に効果的なハンドマッサージ法、美味しいハーブティの淹れ方など、健康に役立つ知識を習得しましょう。
+◆対象
+・自分に合った自然治癒力を高める方法を学びたい方</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>品川区</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>昭和医科大学リカレントカレッジ</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>16名</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>12,000円</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>2025年12月20日（土）</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>154590</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>その他医療・福祉,対面講座</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>2025-12-23</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>自ら学ぶ“自ら守る”おとなのアレルギー・アナフィラキシーショック</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/154590</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>アナフィラキシーショックは生命を脅かす可能性がある最重症の急性アレルギー反応です。
+医療従事者にとっては学修必須の病態ですが、一般の方向けで特に成人を対象に上記をテーマとした教育の機会が開講されることは稀少であるのが現状です。
+本講座では、アレルギー疾患の有無を問わず、周囲で発症した者がいた際に注意すべきことや、緊急対処方法などについて学修していきます。
+◆対象
+・自身に食物アレルギーや薬剤アレルギーがあり、アナフィラキシーショックに関する医学知識や最新の知見を学びたい方
+・家族や友人など周囲にアナフィラキシーショックの既往があり、緊急対処方法やケアの仕方を学びたい方
+・成人のアレルギー疾患について学びたい方</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>品川区</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>昭和医科大学リカレントカレッジ</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>16名</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>15,000円</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>2025年11月20日（木）</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>154586</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>その他カルチャー,オンライン講座</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>2025-12-02</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>マインドフルネスストレス低減法(MBSR)8週間コース</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/154586</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>マインドフルネスストレス低減法(Mindfulness-Based Stress Reduction: MBSR)は、ジョン・カバットジン博士(Jon Kabat-Zinn)が1979年にマサチューセッツ大学メディカルセンターで開発したストレスマネジメントプログラムです。慢性疼痛の症状軽減や心身のストレス反応を和らげる効果が認められ、現在では、医療、福祉、教育、企業など、様々な分野で応用されています。
+本講座では、インターナショナルマインドフルネスセンタージャパン(IMCJ)の研修を修了した講師とともに、MBSR8週間コースを体系的に学び、日常生活で実践できるスキルを身につけることを目指します。仕事や人間関係などにおけるストレスへの向き合い方を見直し、健やかで充実した日々を送りたい方に最適なプログラムです。この機会に、マインドフルネスの実践をしながら心と体の調和を取り戻してみませんか?
+◆対象
+・日常生活や仕事上のストレスを減らしたい方
+・心身のバランスを整えて、充実した日々を過ごしたい方
+・対話力を育てて、人間関係の改善を望む方
+・マインドフルネスという言葉を知っていて、実践する機会を探している方</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
           <t>オンライン</t>
         </is>
       </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>東京都</t>
-        </is>
-      </c>
-      <c r="I30" t="inlineStr">
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>昭和医科大学リカレントカレッジ</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>12名</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>35,000円</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>2025年11月20日（木）</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>154583</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>経済,産業,社会,オンライン講座,対面講座</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>2025-11-27</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>海を越えた犯罪者たち ～国際犯罪の実態に迫る～</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/154583</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>カルロス・ゴーンが海外に逃亡した事件をご記憶されている方も多いと思います。このように海外に逃亡した犯人を我が国に連れ戻して裁判をすることはできないのでしょうか。同人は、現在も海外で優雅に暮らしているようですが、そのような事態は、実は少なくないのです。なぜそのようなことが起きてしまうのか、法はどのような対処方法を用意しているのか、また、その限界はどこにあるのかなどについて具体的に解説いたします。
+◆対象
+・犯罪や捜査などの法律問題に興味のある方
+・国際犯罪への法の対処に興味がある方</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>オンライン,品川区</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>昭和医科大学リカレントカレッジ</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>20名</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>16,000円</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>2025年10月20日（月）</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>154574</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>その他医療・福祉,オンライン講座,対面講座</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>2025-11-21</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>生活習慣を見直して健康寿命を延ばそう!</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/154574</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>2000年に策定された「健康日本21」では健康寿命を延ばすため、生活習慣病予防に重点を置いています。生活習慣を改善することは容易ではありません。まずは関心を持っていただくことが第一歩となります。飲酒、喫煙、コーヒー飲用、ウォーキング・身体活動、睡眠などの生活習慣と高血圧症、糖尿病などの生活習慣病との関連についての研究結果をわかりやすく伝えていきます。ご自身の生活習慣を見つめなおしてみませんか?
+◆対象
+・自らの生活習慣を見直したい一般の方
+・予防医学に興味がある一般の方
+・疫学に興味がある一般の方</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>オンライン,品川区</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>昭和医科大学リカレントカレッジ</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>20名</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>15,000円</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>2025年10月20日（月）</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>154570</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>その他カルチャー,対面講座</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>2025-11-12</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>スマホで秋を撮る ～感性を豊かにする山歩(さんぽ) ～</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/154570</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>スマホの登場で写真を撮ることがとても身近になりました。写真を撮るという行為は、なんとなく撮影してしまえばそれまでですが、ひと手間かけてあげることで素晴らしい作品となります。また、撮影する際に気に入った被写体を探す動作や構図を考える作業は、良い脳への刺激となります。本講座では、座学と撮影会・講評会を通して、日常の風景を美しく切り取る技術を学び実践するとともに、写真を撮ることが健康へ与える影響を学びます。リピーターの方には光の使い方などより高度な技術を学んでいただくこともできます。
+◆対象
+・写真撮影に興味がある方
+・スマホ、一眼カメラでの写真撮影に興味がある方
+・写真撮影の基礎を学びたい方
+・自然やハイキングが好きな方
+・芸術が脳へ及ぼす影響に興味がある方</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>品川区</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>昭和医科大学リカレントカレッジ</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>10名</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>15,000円</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>2025年10月20日（月）</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>154557</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>その他カルチャー,対面講座</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>2025-11-05</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>秋の夜長を楽しむヨガ ～ヨガの基礎理論と実践～</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/154557</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>ヨガは単なる運動ではなく、歴史や哲学を持つ奥深い実践法であり、近年、医療やヘルスケアの現場において、ヨガがもたらす心身の健康効果が注目されています。
+本講座では、ヨガの起源や哲学、さまざまな流派の特徴を学びながら、ヨガと健康に関する最新の臨床研究も紹介し、科学的な視点からその効果を探ります。また、知識を深めるだけでなく、各流派のヨガを実際に体験する実習を取り入れ、理論と実践をバランスよく学べる構成としています。ヨガの実践を始めてみたい方、心身の健康を維持したい方、新しい学びやライフワークを探している方に最適な講座です。身体を動かしながら、ヨガの本質を学び、より豊かな人生を築いてみませんか?
+◆対象・これからヨガの実践を始めてみたい方
+・ヨガに関する基本的な知識を体系的に勉強してみたい方
+・自分自身に適したヨガのスタイルを探したいと思っている方
+・心身の健康を維持したい方</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>品川区</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>昭和医科大学リカレントカレッジ</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>12名</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>12,000円</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>2025年10月20日（月）</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>154277</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>その他経済産業・社会,オンデマンド講座</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>2025-10-01</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>【アーカイブ】公共政策リスキリング講座Ⅱ</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/154277</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>本講座は，公共政策リスキリング講座として開設するものであり，行政と何らかの関りを持つ人や公共政策に関心を有する人を対象とし，国・自治体が実施する公共政策について，その背景となる社会事情や制度を講師が解説し，新たな視点から公共政策を考えてみることを目的とする講座である。
+住民に身近な法制度を，住民のためにどのように利用していくべきなのか？このシリーズは，このような問題意識の下で，「入門 行政法と地方自治法」というテーマを設定した。専門的な予備知識は必要とせず，行政の仕事に関心を持つ人であれば誰でも理解できる内容を提供する。
+市民の日常生活は様々な行政サービスに取り囲まれているが，行政サービスの基礎的なフレームとなるのは法制度である。そしてその中でも最も広範に住民生活と結びついている法分野は，個別行政法の基礎となる行政法と地方自治法である。そこで，本講座では，行政法では具体的な紛争となることも多い行政指導，地方自治法関連では，条例，住民訴訟及び住民投票の３つをテーマとして採り上げる。
+第１回は，「行政指導の何が問題なのか？」をテーマとする。行政指導は，我が国では高度に練り上げられた行政手法であるが，この用語自体がネガティブなイメージで用いられることも多い。それでは何が問題になっているのか，問題点を踏まえて，市民は行政機関に何を求めればよいのか，行政機関はどのような点に留意するべきなのか等の点について考えてみる。
+第2回は，「条例とはどのように創るのか？」をテーマとする。現在，条例は自治体の執行機関により立案され議会に提案されることが多いが，自治体はどのような発想や手順で条例を立案しているのか。また，地方自治法の直接請求に基づいて市民が条例を立案することも可能であるが，どのような点に留意するべきなのか等について考えてみる。
+第3回は，「住民訴訟」をテーマとする。住民訴訟は納税者訴訟とも呼ばれ，市民の視点から自治体の支出の適正性を求めることを通じ，自治体の行政活動をチェックする仕組みである。我が国で盛んに活用されている現状を踏まえ，住民自治の観点から，どのような制度活用が最も効果的であるのか等の点を考える。
+第4回は，「住民投票」をテーマとする。現在，条例に基づく住民投票は盛んに活用されているが，どのようなテーマに対し，住民投票制度は最も効果的に活用し得るのか，及び自治体としてはどのように制度を運用していくことが中長期的な住民の便益に資するのかという点を中心に，今後の制度運用を考える。
+配信期間：2025年10月1日(水)～2026年3月31日(火)</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>オンライン</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>明治大学</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>4,400円</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>2026年2月18日（水）23:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>154274</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>その他経済産業・社会,オンデマンド講座</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>2025-10-01</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>【アーカイブ】公共政策リスキリング講座Ⅰ</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/154274</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>本講座は，公共政策リスキリング講座として開設するものであり，行政と何らかの関りを持つ人や公共政策に関心を有する人を対象とし，国・自治体が実施する公共政策について，その背景となる社会事情や制度を講師が解説し，新たな視点から公共政策を考えてみることを目的とする講座である。専門的な予備知識は必要とせず，行政の仕事に関心を持つ人であれば誰でも理解できる内容を提供する。
+今日，コロナや急激な人口減少という未経験の社会現象に直面し，地域で生活を送る住民の心も揺れている。このような中で，持続可能な地域づくりをどのように進めていくべきなのか？このシリーズは，このような問題意識の下で，「SDGsとまちづくり」というテーマを設定した。
+第１回は，「公共ファシリティマネジメントとは？（公共施設の将来を考える。）」をテーマとする。人口減少が進む中で，自治体は，学校，市民ホールその他の公共施設の総量を維持することが困難になり，公共施設の再配置というコンセプトの下で，公共施設の複合化，転用又は処分に取り組んでいる。このような状況の下で，住民自身の視点から公共施設のマネジメントを考える。
+第2回は，「コンパクトシティ」をテーマとする。現在，多くの自治体において，よりコンパクトなゾーンを設定し都市の機能を収斂させていく施策の取組が行われている。このような立地適正化や地域公共交通との連携に焦点を当て，持続的発展を目指した政策の今後を考えてみる。
+第3回は，「地域公共交通とまちづくり」をテーマとし，地域の持続的発展と地域公共交通のあり方に焦点を当てる。具体的には，コミュニティバス等の車両系の交通整備の在り方と，地域鉄道の再編を含む鉄道系の交通整備の在り方について考えてみる。
+第4回は，「グリーンボンド（環境債）とまちづくり」をテーマとする。具体的には，我が国におけるグリーンボンドの取組に焦点を当て，ESG投資にみられるような社会的インパクト，地球環境問題，及び地域の持続的発展のような新しいコンセプトと自治体のまちづくりについて考えてみる。
+配信期間：2025年10月1日(水)～2026年3月31日(火)</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>オンライン</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>明治大学</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>4,400円</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>2026年2月18日（水）23:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>154271</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>その他ビジネススキル,オンデマンド講座</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>2025-10-01</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>【アーカイブ】Excelで学ぶ実務データの分析</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/154271</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>ビジネスの世界では、企業の経営判断、事業評価などを行う局面において、データ分析による客観的な数値を基にした評価が不可欠となっている。そして、こうした業務を担う、データ・サイエンティストと呼ばれる人材が益々重要な時代になってきている。本講座では、「経営を見える化する」ために、データをどのように集め、加工し、データ分析を行うことで、最終的にどのように判断するのかという一連の流れをExcelの分析ツールを用いた実習によって解説する。
+入門講座であり、理論の解説よりも実践に必要な理論の適用法を中心に説明する。数学的な前提は必要としないが、実習に対応するためExcelの基本はマスターしていることを前提としている。
+配信期間：2025年10月1日(水)～2026年3月31日(火)</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>オンライン</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>明治大学</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>5,500円</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>2026年2月18日（水）23:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>154268</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>その他ビジネススキル,オンデマンド講座</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>2025-10-01</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>【アーカイブ】Excelで学ぶデータ解析入門</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/154268</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>ビジネスの世界では、企業の経営判断、事業評価などを行う局面において、データ解析よる客観的な数値による評価が不可欠となっている。そして、こうした業務を担う、データ・サイエンティストと呼ばれる人材が益々重要な時代になってきている。本講座では、「経営を見える化する」ために、データをどのように集め、加工し、データ解析を行うことで、最終的にどのように判断するのかという一連の流れをExcelの分析ツールを用いた実習によって解説する。入門講座であり、理論の解説よりも実践に必要な理論の適用法を中心に説明する。
+数学的な前提は必要としないが、実習に対応するためExcelの基本はマスターしていることを前提とする。
+配信期間：2025年10月1日(水)～2026年3月31日(火)</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>オンライン</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>明治大学</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>5,500円</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>2026年2月18日（水）23:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>154265</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>経営,オンデマンド講座</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>2025-10-01</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>【アーカイブ】経営学余話シリーズPart5</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/154265</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>人生が私たちの生活であるならば、経営は企業にとっての生活にほかなりません。本講座では、経営、企業といった身近な事象や存在について、経営学の名著をとおして、いまいちど見直し、再考することで、その本質や実像に迫りたいと思います。
+今回も経営学余話シリーズの第5弾として、知っていそうであまり知られていない経営に関わる身近な事がらをピックアップして、皆さんとご一緒に掘り下げてみたいと思います。
+配信期間：2025年10月1日(水)～2026年3月31日(火)</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>オンライン</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>明治大学</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>5,500円</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>2026年2月18日（水）23:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>154262</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>経営,オンデマンド講座</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>2025-10-01</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>【アーカイブ】経営学余話シリーズPart4</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/154262</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>人生が私たちの生活であるならば、経営は企業にとっての生活にほかなりません。日々の生活に努力するのと同じように、企業も自らの経営に大きな努力を払っています。
+本講座では、「企業ってなに？」「経営ってなにをすることなの？」といったはじまりの話から、企業経営に関する秘話、とっておきのお話、感動の物語についてみなさんとご一緒に触れてみたいと思います。学問として「経営」といった難しい話ではなく、経営に関する「雑学」についてご紹介したいと思います。
+今回も経営学余話シリーズの第4弾として、知っていそうであまり知られていない経営に関わる身近な事がらをピックアップして、皆さんとご一緒に掘り下げてみたいと思います。
+配信期間：2025年10月1日(水)～2026年3月31日(火)</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>オンライン</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>明治大学</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>5,500円</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>2026年2月18日（水）23:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>154259</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>経済,経営,歴史・哲学,オンデマンド講座</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>2025-10-01</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>【アーカイブ】経営学余話シリーズPart3</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/154259</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>江戸後期を起点とする日本の経済の近代化と、それを支えてきた経営体について、明治から令和におよぶ一世紀半の時空に隠れた余話の紹介を内容とします。
+　戦時および戦後の経済動乱、高度経済成長、バブル経済、リーマンショック、東日本大震災、そして新型コロナショック等々、よく耳にはするものの、それらの発生要因とその後への影響、そしてそこに起きていた事実などを深く知ることはあまりないようです。そうした時代の転換点におけるドラマの平易な紹介をとおして、日本の経済と経営の歴史を振り返ってみたいと思います。
+配信期間：2025年10月1日(水)～2026年3月31日(火)</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>オンライン</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>明治大学</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>5,500円</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>2026年2月18日（水）23:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="inlineStr">
+        <is>
+          <t>154256</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>経済,経営,歴史・哲学,オンデマンド講座</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>2025-10-01</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>【アーカイブ】経営学余話シリーズPart2</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/154256</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>江戸後期を起点とする日本の経済の近代化と、それを支えてきた経営体について、明治から令和におよぶ一世紀半の時空に隠れた余話の紹介を内容とします。
+　戦時および戦後の経済動乱、高度経済成長、バブル経済、リーマンショック、東日本大震災、そして新型コロナショック等々、よく耳にはするものの、それらの発生要因とその後への影響、そしてそこに起きていた事実などを深く知ることはあまりないようです。そうした時代の転換点におけるドラマの平易な紹介をとおして、日本の経済と経営の歴史を振り返ってみたいと思います。
+配信期間：2025年10月1日(水)～2026年3月31日(火)</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>オンライン</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>明治大学</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>5,500円</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>2026年2月18日（水）23:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="inlineStr">
+        <is>
+          <t>154253</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>経営,オンデマンド講座</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>2025-10-01</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>【アーカイブ】経営学余話シリーズPart1</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/154253</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>人生が私たちの生活であるならば、経営は企業にとっての生活にほかなりません。日々の生活に努力するのと同じように、企業も自らの経営に大きな努力を払っています。
+　本講座では、「企業ってなに？」「経営ってなにをすることなの？」といったはじまりの話から、企業経営に関する秘話、とっておきのお話、感動の物語についてみなさんとご一緒に触れてみたいと思います。学問として「経営」といった難しい話ではなく、経営に関する「雑学」についてご紹介したいと思います。
+配信期間：2025年10月1日(水)～2026年3月31日(火)</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>オンライン</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>明治大学</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>5,500円</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>2026年2月18日（水）23:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="inlineStr">
+        <is>
+          <t>154248</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>その他経済産業・社会,オンライン講座</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>2026-03-03</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>【ハイブリッド】地方自治と行政法</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/154248</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>地方公務員を対象に、行政法の基本的な考え方を地方行政の実務に即して解説することを通じ、行政実務に通底する法律的な考え方を構造的に理解することが可能となり、行政実務の習熟に貢献することができる。具体的には、「法律による行政の原理とは？」「行政行為とは？」「行政指導とは？及び「国家賠償制度とは？」という４つのポイントを設定し、行政実務に即したわかり易い解説を行う。</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>オンライン,千代田区</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>明治大学</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>100名</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>15,200円</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>2026年2月20日（金）23:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="inlineStr">
+        <is>
+          <t>153682</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>歴史・哲学,オンデマンド講座</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>2026-03-07</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>【ハイブリッド/オンデマンド】 小栗忠順の生涯－時代を先読みした幕臣－ 《明治大学連合駿台会寄付講座》</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>https://www.recurrent-navi.metro.tokyo.lg.jp/course/153682</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>2027年NHK大河ドラマの主人公となった小栗上野介忠順は、現在の千代田区神田駿河台（本学駿河台キャンパス近隣）に生まれ、1860年（万延元年）に遣米使節の目付役として渡米、世界を一周して帰国後、幕府の要職に就き日本の近代化に奔走しました。
+本講座では小栗の生涯を、ご紹介いたします。
+配信期日（予定）：
+2026年3月31日（土）
+※24時間視聴可能</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>オンライン</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>明治大学</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
         <is>
           <t>なし</t>
         </is>
       </c>
-      <c r="J30" t="inlineStr">
+      <c r="J51" t="inlineStr">
         <is>
           <t>無料</t>
         </is>
       </c>
-      <c r="K30" t="inlineStr">
-        <is>
-          <t>なし</t>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>2026年3月6日（金）23:59</t>
         </is>
       </c>
     </row>

</xml_diff>